<commit_message>
Update master_data.xlsx with 3XO PETROL 08/07/2025
</commit_message>
<xml_diff>
--- a/data/master_data.xlsx
+++ b/data/master_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,6 +721,942 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>3XO PETROL</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>